<commit_message>
added core course info (pulled from programs CSV)
</commit_message>
<xml_diff>
--- a/ingest/resources/programs-list-2016-04-24_20.27.21.xlsx
+++ b/ingest/resources/programs-list-2016-04-24_20.27.21.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/szednik/Sites/rpinfo2/ingest/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="1114">
   <si>
     <t>Organization OID</t>
   </si>
@@ -21204,14 +21216,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -21222,28 +21229,34 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -21533,19 +21546,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="64.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -21598,7 +21625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -21642,7 +21669,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -21686,7 +21713,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -21724,7 +21751,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -21768,7 +21795,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -21815,7 +21842,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -21859,7 +21886,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>17</v>
       </c>
@@ -21906,7 +21933,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -21950,7 +21977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -21991,7 +22018,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>17</v>
       </c>
@@ -22038,7 +22065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -22085,7 +22112,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -22132,7 +22159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -22179,7 +22206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>17</v>
       </c>
@@ -22226,7 +22253,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>17</v>
       </c>
@@ -22273,7 +22300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -22320,7 +22347,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -22367,7 +22394,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -22411,7 +22438,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -22449,7 +22476,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>17</v>
       </c>
@@ -22493,7 +22520,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -22534,7 +22561,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>17</v>
       </c>
@@ -22581,7 +22608,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>17</v>
       </c>
@@ -22622,7 +22649,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>17</v>
       </c>
@@ -22666,7 +22693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>17</v>
       </c>
@@ -22707,7 +22734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>17</v>
       </c>
@@ -22751,7 +22778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -22795,7 +22822,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>17</v>
       </c>
@@ -22839,7 +22866,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>17</v>
       </c>
@@ -22883,7 +22910,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -22927,7 +22954,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>17</v>
       </c>
@@ -22971,7 +22998,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>17</v>
       </c>
@@ -23018,7 +23045,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>17</v>
       </c>
@@ -23065,7 +23092,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>17</v>
       </c>
@@ -23112,7 +23139,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>17</v>
       </c>
@@ -23153,7 +23180,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>17</v>
       </c>
@@ -23200,7 +23227,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>17</v>
       </c>
@@ -23247,7 +23274,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>17</v>
       </c>
@@ -23291,7 +23318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>17</v>
       </c>
@@ -23332,7 +23359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>17</v>
       </c>
@@ -23379,7 +23406,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>17</v>
       </c>
@@ -23423,7 +23450,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>17</v>
       </c>
@@ -23464,7 +23491,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>17</v>
       </c>
@@ -23511,7 +23538,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>17</v>
       </c>
@@ -23558,7 +23585,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>17</v>
       </c>
@@ -23605,7 +23632,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>17</v>
       </c>
@@ -23649,7 +23676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>17</v>
       </c>
@@ -23696,7 +23723,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>17</v>
       </c>
@@ -23743,7 +23770,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>17</v>
       </c>
@@ -23790,7 +23817,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>17</v>
       </c>
@@ -23837,7 +23864,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>17</v>
       </c>
@@ -23878,7 +23905,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>17</v>
       </c>
@@ -23925,7 +23952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>17</v>
       </c>
@@ -23969,7 +23996,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>17</v>
       </c>
@@ -24013,7 +24040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>17</v>
       </c>
@@ -24060,7 +24087,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>17</v>
       </c>
@@ -24107,7 +24134,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>17</v>
       </c>
@@ -24154,7 +24181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>17</v>
       </c>
@@ -24201,7 +24228,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>17</v>
       </c>
@@ -24245,7 +24272,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>17</v>
       </c>
@@ -24286,7 +24313,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>17</v>
       </c>
@@ -24333,7 +24360,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>17</v>
       </c>
@@ -24380,7 +24407,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>17</v>
       </c>
@@ -24427,7 +24454,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>17</v>
       </c>
@@ -24474,7 +24501,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>17</v>
       </c>
@@ -24518,7 +24545,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>17</v>
       </c>
@@ -24559,7 +24586,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>17</v>
       </c>
@@ -24606,7 +24633,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>17</v>
       </c>
@@ -24653,7 +24680,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>17</v>
       </c>
@@ -24694,7 +24721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>17</v>
       </c>
@@ -24738,7 +24765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>17</v>
       </c>
@@ -24785,7 +24812,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>17</v>
       </c>
@@ -24829,7 +24856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>17</v>
       </c>
@@ -24876,7 +24903,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>17</v>
       </c>
@@ -24923,7 +24950,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>17</v>
       </c>
@@ -24970,7 +24997,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>17</v>
       </c>
@@ -25014,7 +25041,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>17</v>
       </c>
@@ -25061,7 +25088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>17</v>
       </c>
@@ -25108,7 +25135,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>17</v>
       </c>
@@ -25155,7 +25182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>17</v>
       </c>
@@ -25199,7 +25226,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>17</v>
       </c>
@@ -25243,7 +25270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>17</v>
       </c>
@@ -25287,7 +25314,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>17</v>
       </c>
@@ -25331,7 +25358,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>17</v>
       </c>
@@ -25378,7 +25405,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>17</v>
       </c>
@@ -25425,7 +25452,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>17</v>
       </c>
@@ -25469,7 +25496,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>17</v>
       </c>
@@ -25516,7 +25543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>17</v>
       </c>
@@ -25563,7 +25590,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>17</v>
       </c>
@@ -25604,7 +25631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>17</v>
       </c>
@@ -25648,7 +25675,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>17</v>
       </c>
@@ -25695,7 +25722,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>17</v>
       </c>
@@ -25742,7 +25769,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>17</v>
       </c>
@@ -25789,7 +25816,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>17</v>
       </c>
@@ -25833,7 +25860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="96" spans="1:17">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>17</v>
       </c>
@@ -25880,7 +25907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17">
+    <row r="97" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>17</v>
       </c>
@@ -25927,7 +25954,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="98" spans="1:17">
+    <row r="98" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>17</v>
       </c>
@@ -25974,7 +26001,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="99" spans="1:17">
+    <row r="99" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>17</v>
       </c>
@@ -26018,7 +26045,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
+    <row r="100" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>17</v>
       </c>
@@ -26062,7 +26089,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="101" spans="1:17">
+    <row r="101" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>17</v>
       </c>
@@ -26106,7 +26133,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>17</v>
       </c>
@@ -26153,7 +26180,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="103" spans="1:17">
+    <row r="103" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>17</v>
       </c>
@@ -26197,7 +26224,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
+    <row r="104" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>17</v>
       </c>
@@ -26244,7 +26271,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="105" spans="1:17">
+    <row r="105" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>17</v>
       </c>
@@ -26288,7 +26315,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>17</v>
       </c>
@@ -26335,7 +26362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>17</v>
       </c>
@@ -26382,7 +26409,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
+    <row r="108" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>17</v>
       </c>
@@ -26429,7 +26456,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="109" spans="1:17">
+    <row r="109" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>17</v>
       </c>
@@ -26470,7 +26497,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>17</v>
       </c>
@@ -26517,7 +26544,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="111" spans="1:17">
+    <row r="111" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>17</v>
       </c>
@@ -26561,7 +26588,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:17">
+    <row r="112" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>17</v>
       </c>
@@ -26608,7 +26635,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>17</v>
       </c>
@@ -26649,7 +26676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>17</v>
       </c>
@@ -26693,7 +26720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>17</v>
       </c>
@@ -26737,7 +26764,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>17</v>
       </c>
@@ -26781,7 +26808,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>17</v>
       </c>
@@ -26825,7 +26852,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>17</v>
       </c>
@@ -26869,7 +26896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>17</v>
       </c>
@@ -26916,7 +26943,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>17</v>
       </c>
@@ -26957,7 +26984,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="121" spans="1:17">
+    <row r="121" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>17</v>
       </c>
@@ -27004,7 +27031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="122" spans="1:17">
+    <row r="122" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>17</v>
       </c>
@@ -27051,7 +27078,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:17">
+    <row r="123" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>17</v>
       </c>
@@ -27098,7 +27125,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="124" spans="1:17">
+    <row r="124" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>17</v>
       </c>
@@ -27145,7 +27172,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:17">
+    <row r="125" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>17</v>
       </c>
@@ -27186,7 +27213,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="126" spans="1:17">
+    <row r="126" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>17</v>
       </c>
@@ -27233,7 +27260,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="127" spans="1:17">
+    <row r="127" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>17</v>
       </c>
@@ -27280,7 +27307,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="128" spans="1:17">
+    <row r="128" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>17</v>
       </c>
@@ -27327,7 +27354,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="129" spans="1:17">
+    <row r="129" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>17</v>
       </c>
@@ -27368,7 +27395,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="130" spans="1:17">
+    <row r="130" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>17</v>
       </c>
@@ -27415,7 +27442,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="131" spans="1:17">
+    <row r="131" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>17</v>
       </c>
@@ -27462,7 +27489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="132" spans="1:17">
+    <row r="132" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>17</v>
       </c>
@@ -27503,7 +27530,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="133" spans="1:17">
+    <row r="133" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>17</v>
       </c>
@@ -27547,7 +27574,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="134" spans="1:17">
+    <row r="134" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>17</v>
       </c>
@@ -27594,7 +27621,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="135" spans="1:17">
+    <row r="135" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>17</v>
       </c>
@@ -27641,7 +27668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:17">
+    <row r="136" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>17</v>
       </c>
@@ -27685,7 +27712,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="137" spans="1:17">
+    <row r="137" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>17</v>
       </c>
@@ -27732,7 +27759,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="138" spans="1:17">
+    <row r="138" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>17</v>
       </c>
@@ -27779,7 +27806,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="139" spans="1:17">
+    <row r="139" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>17</v>
       </c>
@@ -27826,7 +27853,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="140" spans="1:17">
+    <row r="140" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>17</v>
       </c>
@@ -27870,7 +27897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
+    <row r="141" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>17</v>
       </c>
@@ -27914,7 +27941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="142" spans="1:17">
+    <row r="142" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>17</v>
       </c>
@@ -27955,7 +27982,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="143" spans="1:17">
+    <row r="143" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>17</v>
       </c>
@@ -28002,7 +28029,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="144" spans="1:17">
+    <row r="144" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>17</v>
       </c>
@@ -28046,7 +28073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="1:17">
+    <row r="145" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>17</v>
       </c>
@@ -28090,7 +28117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="146" spans="1:17">
+    <row r="146" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>17</v>
       </c>
@@ -28131,7 +28158,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="147" spans="1:17">
+    <row r="147" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>17</v>
       </c>
@@ -28178,7 +28205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="148" spans="1:17">
+    <row r="148" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>17</v>
       </c>
@@ -28219,7 +28246,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="149" spans="1:17">
+    <row r="149" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>17</v>
       </c>
@@ -28266,7 +28293,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="150" spans="1:17">
+    <row r="150" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>17</v>
       </c>
@@ -28313,7 +28340,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="151" spans="1:17">
+    <row r="151" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>17</v>
       </c>
@@ -28354,7 +28381,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="152" spans="1:17">
+    <row r="152" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>17</v>
       </c>
@@ -28401,7 +28428,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="153" spans="1:17">
+    <row r="153" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>17</v>
       </c>
@@ -28448,7 +28475,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="154" spans="1:17">
+    <row r="154" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>17</v>
       </c>
@@ -28495,7 +28522,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="155" spans="1:17">
+    <row r="155" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>17</v>
       </c>
@@ -28542,7 +28569,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="156" spans="1:17">
+    <row r="156" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>17</v>
       </c>
@@ -28589,7 +28616,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="157" spans="1:17">
+    <row r="157" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>17</v>
       </c>
@@ -28636,7 +28663,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="158" spans="1:17">
+    <row r="158" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>17</v>
       </c>
@@ -28683,7 +28710,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="159" spans="1:17">
+    <row r="159" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>17</v>
       </c>
@@ -28730,7 +28757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="160" spans="1:17">
+    <row r="160" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>17</v>
       </c>
@@ -28777,7 +28804,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="161" spans="1:17">
+    <row r="161" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>17</v>
       </c>
@@ -28824,7 +28851,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="162" spans="1:17">
+    <row r="162" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>17</v>
       </c>
@@ -28868,7 +28895,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="163" spans="1:17">
+    <row r="163" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>17</v>
       </c>
@@ -28912,7 +28939,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="164" spans="1:17">
+    <row r="164" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>17</v>
       </c>
@@ -28959,7 +28986,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="165" spans="1:17">
+    <row r="165" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>17</v>
       </c>
@@ -29003,7 +29030,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="166" spans="1:17">
+    <row r="166" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>17</v>
       </c>
@@ -29047,7 +29074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="167" spans="1:17">
+    <row r="167" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>17</v>
       </c>
@@ -29091,7 +29118,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="168" spans="1:17">
+    <row r="168" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
         <v>17</v>
       </c>
@@ -29138,7 +29165,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="169" spans="1:17">
+    <row r="169" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>17</v>
       </c>
@@ -29185,7 +29212,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="170" spans="1:17">
+    <row r="170" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>17</v>
       </c>
@@ -29232,7 +29259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="171" spans="1:17">
+    <row r="171" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>17</v>
       </c>
@@ -29279,7 +29306,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="172" spans="1:17">
+    <row r="172" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>17</v>
       </c>
@@ -29326,7 +29353,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:17">
+    <row r="173" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>17</v>
       </c>
@@ -29373,7 +29400,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="174" spans="1:17">
+    <row r="174" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
         <v>17</v>
       </c>
@@ -29411,7 +29438,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="175" spans="1:17">
+    <row r="175" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>17</v>
       </c>
@@ -29455,7 +29482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="176" spans="1:17">
+    <row r="176" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>17</v>
       </c>
@@ -29499,7 +29526,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="177" spans="1:17">
+    <row r="177" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>17</v>
       </c>
@@ -29537,7 +29564,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="178" spans="1:17">
+    <row r="178" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>17</v>
       </c>
@@ -29581,7 +29608,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="179" spans="1:17">
+    <row r="179" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
         <v>17</v>
       </c>
@@ -29625,7 +29652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="180" spans="1:17">
+    <row r="180" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>17</v>
       </c>
@@ -29672,7 +29699,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="181" spans="1:17">
+    <row r="181" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>17</v>
       </c>
@@ -29719,7 +29746,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="182" spans="1:17">
+    <row r="182" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>17</v>
       </c>
@@ -29763,7 +29790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="183" spans="1:17">
+    <row r="183" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>17</v>
       </c>
@@ -29807,7 +29834,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="184" spans="1:17">
+    <row r="184" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>17</v>
       </c>
@@ -29848,7 +29875,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="185" spans="1:17">
+    <row r="185" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>17</v>
       </c>
@@ -29895,7 +29922,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="186" spans="1:17">
+    <row r="186" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>17</v>
       </c>
@@ -29939,7 +29966,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="187" spans="1:17">
+    <row r="187" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>17</v>
       </c>
@@ -29986,7 +30013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="188" spans="1:17">
+    <row r="188" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
         <v>17</v>
       </c>
@@ -30030,7 +30057,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="189" spans="1:17">
+    <row r="189" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>17</v>
       </c>
@@ -30077,7 +30104,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="190" spans="1:17">
+    <row r="190" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>17</v>
       </c>
@@ -30121,7 +30148,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="191" spans="1:17">
+    <row r="191" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
         <v>17</v>
       </c>
@@ -30165,7 +30192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:17">
+    <row r="192" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>17</v>
       </c>
@@ -30212,7 +30239,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:17">
+    <row r="193" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>17</v>
       </c>
@@ -30259,7 +30286,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="194" spans="1:17">
+    <row r="194" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>17</v>
       </c>
@@ -30303,7 +30330,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="195" spans="1:17">
+    <row r="195" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>17</v>
       </c>
@@ -30347,7 +30374,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="196" spans="1:17">
+    <row r="196" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>17</v>
       </c>
@@ -30394,7 +30421,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="197" spans="1:17">
+    <row r="197" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
         <v>17</v>
       </c>
@@ -30441,7 +30468,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="198" spans="1:17">
+    <row r="198" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>17</v>
       </c>
@@ -30488,7 +30515,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="199" spans="1:17">
+    <row r="199" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>17</v>
       </c>
@@ -30532,7 +30559,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="200" spans="1:17">
+    <row r="200" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>17</v>
       </c>
@@ -30573,7 +30600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="201" spans="1:17">
+    <row r="201" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>17</v>
       </c>
@@ -30617,7 +30644,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="202" spans="1:17">
+    <row r="202" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
         <v>17</v>
       </c>
@@ -30658,7 +30685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="203" spans="1:17">
+    <row r="203" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
         <v>17</v>
       </c>
@@ -30702,7 +30729,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="204" spans="1:17">
+    <row r="204" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
         <v>17</v>
       </c>
@@ -30746,7 +30773,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="205" spans="1:17">
+    <row r="205" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
         <v>17</v>
       </c>
@@ -30787,7 +30814,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="206" spans="1:17">
+    <row r="206" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
         <v>17</v>
       </c>
@@ -30831,7 +30858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="207" spans="1:17">
+    <row r="207" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
         <v>17</v>
       </c>
@@ -30875,7 +30902,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="208" spans="1:17">
+    <row r="208" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
         <v>17</v>
       </c>
@@ -30922,7 +30949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="209" spans="1:17">
+    <row r="209" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
         <v>17</v>
       </c>
@@ -30969,7 +30996,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="210" spans="1:17">
+    <row r="210" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
         <v>17</v>
       </c>
@@ -31013,7 +31040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="211" spans="1:17">
+    <row r="211" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
         <v>17</v>
       </c>
@@ -31063,7 +31090,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="212" spans="1:17">
+    <row r="212" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
         <v>17</v>
       </c>
@@ -31107,7 +31134,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="213" spans="1:17">
+    <row r="213" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
         <v>17</v>
       </c>
@@ -31154,7 +31181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="214" spans="1:17">
+    <row r="214" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
         <v>17</v>
       </c>
@@ -31198,7 +31225,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="215" spans="1:17">
+    <row r="215" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
         <v>17</v>
       </c>
@@ -31245,7 +31272,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="216" spans="1:17">
+    <row r="216" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
         <v>17</v>
       </c>
@@ -31292,7 +31319,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="217" spans="1:17">
+    <row r="217" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
         <v>17</v>
       </c>
@@ -31339,7 +31366,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="218" spans="1:17">
+    <row r="218" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
         <v>17</v>
       </c>
@@ -31383,7 +31410,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="219" spans="1:17">
+    <row r="219" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
         <v>17</v>
       </c>
@@ -31424,7 +31451,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="220" spans="1:17">
+    <row r="220" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
         <v>17</v>
       </c>
@@ -31468,7 +31495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="221" spans="1:17">
+    <row r="221" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
         <v>17</v>
       </c>
@@ -31515,7 +31542,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="222" spans="1:17">
+    <row r="222" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
         <v>17</v>
       </c>
@@ -31562,7 +31589,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="223" spans="1:17">
+    <row r="223" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
         <v>17</v>
       </c>
@@ -31609,7 +31636,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="224" spans="1:17">
+    <row r="224" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
         <v>17</v>
       </c>
@@ -31653,7 +31680,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="225" spans="1:17">
+    <row r="225" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
         <v>17</v>
       </c>
@@ -31700,7 +31727,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="226" spans="1:17">
+    <row r="226" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
         <v>17</v>
       </c>
@@ -31748,17 +31775,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>